<commit_message>
ready for first class
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/2019/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F580C48-76F2-564F-9D3A-0F46B10C01D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2795D20B-C09F-7845-9CD9-9537B2B687EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35520" yWindow="-200" windowWidth="27640" windowHeight="14080" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -623,12 +623,6 @@
     <t>Lab: single molecules vs. solution averages</t>
   </si>
   <si>
-    <t>Nelson pp. 82-89, SSTB 7</t>
-  </si>
-  <si>
-    <t>SSTB 5-6, MoL pp. 383-409</t>
-  </si>
-  <si>
     <t>X-ray crystallography (Arden Perkins)</t>
   </si>
   <si>
@@ -707,9 +701,6 @@
     <t>labs/02_pymol/</t>
   </si>
   <si>
-    <t>SSTB 1-4, MoL pp. 294-305</t>
-  </si>
-  <si>
     <t>Kauzmann</t>
   </si>
   <si>
@@ -765,6 +756,15 @@
   </si>
   <si>
     <t>homework/hw7/</t>
+  </si>
+  <si>
+    <t>SSTB 1-3, MoL pp. 294-305</t>
+  </si>
+  <si>
+    <t>SSTB 4-5, MoL pp. 383-409</t>
+  </si>
+  <si>
+    <t>Nelson pp. 82-89, SSTB 6</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1161,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1199,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5" t="s">
@@ -1309,7 +1309,7 @@
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>174</v>
@@ -1333,7 +1333,7 @@
         <v>119</v>
       </c>
       <c r="E6" t="s">
-        <v>195</v>
+        <v>242</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>174</v>
@@ -1354,13 +1354,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
@@ -1417,7 +1417,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s">
         <v>184</v>
@@ -1445,7 +1445,7 @@
         <v>186</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1475,7 +1475,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1504,7 +1504,7 @@
         <v>185</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -1527,7 +1527,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>43</v>
@@ -1566,10 +1566,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>174</v>
@@ -1590,7 +1590,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>174</v>
@@ -1762,7 +1762,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="4" t="s">
@@ -1977,7 +1977,7 @@
         <v>132</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G30" t="s">
         <v>179</v>
@@ -2048,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>190</v>
@@ -2076,50 +2076,50 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2127,39 +2127,39 @@
         <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2167,15 +2167,15 @@
         <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2183,7 +2183,7 @@
         <v>187</v>
       </c>
       <c r="B16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2191,7 +2191,7 @@
         <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2199,7 +2199,7 @@
         <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2207,7 +2207,7 @@
         <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2215,7 +2215,7 @@
         <v>194</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2223,7 +2223,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2231,7 +2231,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2239,7 +2239,7 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2247,7 +2247,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2255,7 +2255,7 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2263,7 +2263,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2271,7 +2271,7 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating schedule with material
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/2019/physical-biochemistry/dev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2795D20B-C09F-7845-9CD9-9537B2B687EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C20552-DC86-E04D-A638-4E4C09968456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="248">
   <si>
     <t>Week</t>
   </si>
@@ -765,13 +765,28 @@
   </si>
   <si>
     <t>Nelson pp. 82-89, SSTB 6</t>
+  </si>
+  <si>
+    <t>01_slides</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/lectures/01_introduction/index.html</t>
+  </si>
+  <si>
+    <t>01_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/01_introduction.pdf</t>
+  </si>
+  <si>
+    <t>01_slides, 01_notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -782,6 +797,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -825,10 +848,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -842,8 +866,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1161,8 +1187,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1255,7 +1281,9 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="G3" t="s">
         <v>175</v>
       </c>
@@ -2046,9 +2074,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -2274,7 +2302,27 @@
         <v>239</v>
       </c>
     </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{E59A957B-636E-984F-96F4-B28CB7BBC29F}"/>
+    <hyperlink ref="B29" r:id="rId2" xr:uid="{3AEC674C-CC9A-324D-B7BE-F8997FED7EE1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added homework 2 and notes
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9829D496-0212-0A49-91D9-854C5D0437A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD74C34-CB1D-2B41-A068-B275CC23CBFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="254">
   <si>
     <t>Week</t>
   </si>
@@ -792,6 +792,12 @@
   </si>
   <si>
     <t>Heat capacity and enthalpy</t>
+  </si>
+  <si>
+    <t>04_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/04_heat-capacity-and-enthalpy.pdf</t>
   </si>
 </sst>
 </file>
@@ -1199,8 +1205,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1380,6 +1386,9 @@
       <c r="E6" t="s">
         <v>240</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>173</v>
       </c>
@@ -2091,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2351,12 +2360,21 @@
         <v>250</v>
       </c>
     </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{E59A957B-636E-984F-96F4-B28CB7BBC29F}"/>
     <hyperlink ref="B29" r:id="rId2" xr:uid="{3AEC674C-CC9A-324D-B7BE-F8997FED7EE1}"/>
     <hyperlink ref="B30" r:id="rId3" xr:uid="{3979A673-1652-AC48-B9E8-AF081DE625A3}"/>
     <hyperlink ref="B31" r:id="rId4" xr:uid="{52C7785C-4E03-264A-8C26-1D093C0D80FA}"/>
+    <hyperlink ref="B32" r:id="rId5" xr:uid="{283D5D72-D312-A840-841B-9E51EB95B8AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hw3, updated schdule, 06_notes
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721119DA-23A4-F24F-8993-351F29ED4B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C47E7C9-5514-1643-B31C-42AF45E95238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="257">
   <si>
     <t>Week</t>
   </si>
@@ -801,6 +801,12 @@
   </si>
   <si>
     <t>https://harmsm.github.io/physical-biochemistry/notes/05_dsc-introduction.pdf</t>
+  </si>
+  <si>
+    <t>06_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/06_protein-folding.pdf</t>
   </si>
 </sst>
 </file>
@@ -1201,8 +1207,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1446,6 +1452,9 @@
       <c r="E8" t="s">
         <v>182</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>255</v>
+      </c>
       <c r="G8" s="4" t="s">
         <v>174</v>
       </c>
@@ -2098,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2374,6 +2383,14 @@
         <v>254</v>
       </c>
     </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>255</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{E59A957B-636E-984F-96F4-B28CB7BBC29F}"/>
@@ -2382,6 +2399,7 @@
     <hyperlink ref="B31" r:id="rId4" xr:uid="{52C7785C-4E03-264A-8C26-1D093C0D80FA}"/>
     <hyperlink ref="B32" r:id="rId5" xr:uid="{283D5D72-D312-A840-841B-9E51EB95B8AD}"/>
     <hyperlink ref="B33" r:id="rId6" xr:uid="{485DE3C5-D6FC-1E43-9E65-70A187335DCB}"/>
+    <hyperlink ref="B34" r:id="rId7" xr:uid="{907580ED-D5D6-254E-A336-E170D77566BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding notes from class 10
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C47E7C9-5514-1643-B31C-42AF45E95238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B28EC7-F448-9949-B1C1-3E18EB92DF30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="259">
   <si>
     <t>Week</t>
   </si>
@@ -807,6 +807,12 @@
   </si>
   <si>
     <t>https://harmsm.github.io/physical-biochemistry/notes/06_protein-folding.pdf</t>
+  </si>
+  <si>
+    <t>10_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/10_structure-based-calcs_sasa.pdf</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1213,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1567,7 +1573,9 @@
       <c r="E12" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>257</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>173</v>
       </c>
@@ -2107,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2391,6 +2399,14 @@
         <v>256</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>257</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{E59A957B-636E-984F-96F4-B28CB7BBC29F}"/>
@@ -2400,6 +2416,7 @@
     <hyperlink ref="B32" r:id="rId5" xr:uid="{283D5D72-D312-A840-841B-9E51EB95B8AD}"/>
     <hyperlink ref="B33" r:id="rId6" xr:uid="{485DE3C5-D6FC-1E43-9E65-70A187335DCB}"/>
     <hyperlink ref="B34" r:id="rId7" xr:uid="{907580ED-D5D6-254E-A336-E170D77566BB}"/>
+    <hyperlink ref="B35" r:id="rId8" xr:uid="{4A6816EE-3597-C74F-9140-B1C790EBA6A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated link in schedule
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677A007C-2CA0-624F-88A1-37FBDA94349D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FE1907-4C78-EA47-8B4E-4855F59E6CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="261">
   <si>
     <t>Week</t>
   </si>
@@ -815,13 +815,10 @@
     <t>https://harmsm.github.io/physical-biochemistry/notes/10_structure-based-calcs_sasa.pdf</t>
   </si>
   <si>
-    <t>10_notes, energetics</t>
-  </si>
-  <si>
     <t>energetics</t>
   </si>
   <si>
-    <t>https://haarmsm.github.io/physical-biochemistry/notes/energy-functions.pdf</t>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/energy-functions.pdf</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1219,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1583,7 +1580,7 @@
         <v>214</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>173</v>
@@ -1613,7 +1610,9 @@
       <c r="E13" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="G13" s="4" t="s">
         <v>177</v>
       </c>
@@ -2126,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2418,10 +2417,10 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>260</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating posted notes, lecture 13
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FE1907-4C78-EA47-8B4E-4855F59E6CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA85092-CA10-0644-BDCC-70DEB72EBBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="265">
   <si>
     <t>Week</t>
   </si>
@@ -819,6 +819,18 @@
   </si>
   <si>
     <t>https://harmsm.github.io/physical-biochemistry/notes/energy-functions.pdf</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/12_electrostatics.pdf</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/13_forcefield-and-sampling.pdf</t>
+  </si>
+  <si>
+    <t>12_notes</t>
+  </si>
+  <si>
+    <t>13_notes</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1231,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1648,6 +1660,9 @@
       <c r="E14" t="s">
         <v>210</v>
       </c>
+      <c r="F14" t="s">
+        <v>263</v>
+      </c>
       <c r="G14" s="4" t="s">
         <v>173</v>
       </c>
@@ -1668,6 +1683,9 @@
       </c>
       <c r="C15" s="4" t="s">
         <v>196</v>
+      </c>
+      <c r="F15" t="s">
+        <v>264</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>173</v>
@@ -2123,10 +2141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2423,6 +2441,22 @@
         <v>260</v>
       </c>
     </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>263</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>264</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{E59A957B-636E-984F-96F4-B28CB7BBC29F}"/>
@@ -2434,6 +2468,8 @@
     <hyperlink ref="B34" r:id="rId7" xr:uid="{907580ED-D5D6-254E-A336-E170D77566BB}"/>
     <hyperlink ref="B35" r:id="rId8" xr:uid="{4A6816EE-3597-C74F-9140-B1C790EBA6A7}"/>
     <hyperlink ref="B36" r:id="rId9" xr:uid="{A37C3867-72C0-A54D-9F6E-9CC921CAAE3C}"/>
+    <hyperlink ref="B37" r:id="rId10" xr:uid="{A6E6DE9B-0046-3E40-98EC-721BA38C12B9}"/>
+    <hyperlink ref="B38" r:id="rId11" xr:uid="{DB0C8733-4F7F-FA4B-9C99-C5EADE371BF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated reading and schedule
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA85092-CA10-0644-BDCC-70DEB72EBBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4D112C-2426-A341-B356-EAEC5B32D53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="270">
   <si>
     <t>Week</t>
   </si>
@@ -831,6 +831,21 @@
   </si>
   <si>
     <t>13_notes</t>
+  </si>
+  <si>
+    <t>readings/binding-methods-and-regression.pdf</t>
+  </si>
+  <si>
+    <t>readings/binding-equations-reference.pdf</t>
+  </si>
+  <si>
+    <t>binding methods</t>
+  </si>
+  <si>
+    <t>binding equations</t>
+  </si>
+  <si>
+    <t>binding methods, binding equations</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1247,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1762,6 +1777,9 @@
       <c r="C18" t="s">
         <v>121</v>
       </c>
+      <c r="E18" t="s">
+        <v>269</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>173</v>
       </c>
@@ -2141,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2455,6 +2473,22 @@
       </c>
       <c r="B38" s="12" t="s">
         <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>267</v>
+      </c>
+      <c r="B39" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added notes for binding
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4D112C-2426-A341-B356-EAEC5B32D53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB011EB-4D97-FB4A-B037-E7E2D883B5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="272">
   <si>
     <t>Week</t>
   </si>
@@ -846,6 +846,12 @@
   </si>
   <si>
     <t>binding methods, binding equations</t>
+  </si>
+  <si>
+    <t>16_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/16_binding-and-itc.pdf</t>
   </si>
 </sst>
 </file>
@@ -1246,8 +1252,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1780,6 +1786,9 @@
       <c r="E18" t="s">
         <v>269</v>
       </c>
+      <c r="F18" t="s">
+        <v>270</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>173</v>
       </c>
@@ -2159,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2489,6 +2498,14 @@
       </c>
       <c r="B40" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2504,6 +2521,7 @@
     <hyperlink ref="B36" r:id="rId9" xr:uid="{A37C3867-72C0-A54D-9F6E-9CC921CAAE3C}"/>
     <hyperlink ref="B37" r:id="rId10" xr:uid="{A6E6DE9B-0046-3E40-98EC-721BA38C12B9}"/>
     <hyperlink ref="B38" r:id="rId11" xr:uid="{DB0C8733-4F7F-FA4B-9C99-C5EADE371BF8}"/>
+    <hyperlink ref="B41" r:id="rId12" xr:uid="{86B48027-D533-B247-B44D-A3AA1E9283CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
posting notes from kinetics iii class
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D0F2CC-B825-964B-B141-36C98A965188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D187823-9023-0D45-AD1D-98271E71707E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="283">
   <si>
     <t>Week</t>
   </si>
@@ -879,6 +879,12 @@
   </si>
   <si>
     <t>19_notes, markov_matrices</t>
+  </si>
+  <si>
+    <t>20_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/20_kinetics-iii.pdf</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1285,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1949,6 +1955,9 @@
       <c r="C23" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="F23" s="4" t="s">
+        <v>281</v>
+      </c>
       <c r="G23" s="4" t="s">
         <v>173</v>
       </c>
@@ -2203,10 +2212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2573,6 +2582,14 @@
       </c>
       <c r="B45" s="12" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>281</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2593,6 +2610,7 @@
     <hyperlink ref="B43" r:id="rId14" xr:uid="{04A669BB-351B-8A4F-BD6E-7AC6A7E14D86}"/>
     <hyperlink ref="B44" r:id="rId15" xr:uid="{1B4A781D-1923-194F-B628-D80AC82F76EA}"/>
     <hyperlink ref="B45" r:id="rId16" xr:uid="{74246AA8-3D05-5D49-A1D1-61AE2FC1268C}"/>
+    <hyperlink ref="B46" r:id="rId17" xr:uid="{37C787D8-404D-9746-B909-B8BD942DF8B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding notes for lecture 21
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D187823-9023-0D45-AD1D-98271E71707E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A6F24-9A31-8D47-8216-4CAADB778714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="285">
   <si>
     <t>Week</t>
   </si>
@@ -885,6 +885,12 @@
   </si>
   <si>
     <t>https://harmsm.github.io/physical-biochemistry/notes/20_kinetics-iii.pdf</t>
+  </si>
+  <si>
+    <t>21_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/21_kinetics-iv.pdf</t>
   </si>
 </sst>
 </file>
@@ -2212,10 +2218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2590,6 +2596,14 @@
       </c>
       <c r="B46" s="12" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>283</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2611,6 +2625,7 @@
     <hyperlink ref="B44" r:id="rId15" xr:uid="{1B4A781D-1923-194F-B628-D80AC82F76EA}"/>
     <hyperlink ref="B45" r:id="rId16" xr:uid="{74246AA8-3D05-5D49-A1D1-61AE2FC1268C}"/>
     <hyperlink ref="B46" r:id="rId17" xr:uid="{37C787D8-404D-9746-B909-B8BD942DF8B1}"/>
+    <hyperlink ref="B47" r:id="rId18" xr:uid="{888CC1C3-1406-B947-895A-D16606A6EBAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
posting hw7, adding lecture 23
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FFB35B-7644-E343-9033-C9C3BDF1DB7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA1B07-FE4F-924F-A84B-368428CF9060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="287">
   <si>
     <t>Week</t>
   </si>
@@ -891,6 +891,12 @@
   </si>
   <si>
     <t>https://mybinder.org/v2/gh/harmsm/kinetics_simulator.git/master?filepath=markov-and-stochastic.ipynb</t>
+  </si>
+  <si>
+    <t>23_notes</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/23_diffusion-i.pdf</t>
   </si>
 </sst>
 </file>
@@ -1291,8 +1297,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2049,6 +2055,9 @@
       <c r="D26" t="s">
         <v>46</v>
       </c>
+      <c r="F26" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="G26" t="s">
         <v>173</v>
       </c>
@@ -2221,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2607,6 +2616,14 @@
       </c>
       <c r="B47" s="12" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2630,6 +2647,7 @@
     <hyperlink ref="B46" r:id="rId17" xr:uid="{37C787D8-404D-9746-B909-B8BD942DF8B1}"/>
     <hyperlink ref="B47" r:id="rId18" xr:uid="{888CC1C3-1406-B947-895A-D16606A6EBAD}"/>
     <hyperlink ref="B19" r:id="rId19" xr:uid="{91AFF295-A0D2-D24C-9DAB-FD4BE8472086}"/>
+    <hyperlink ref="B48" r:id="rId20" xr:uid="{7BC692B1-ADCF-1D4D-BE61-27FE315B3218}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added class 24 notes
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA1B07-FE4F-924F-A84B-368428CF9060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C033D1C2-9AB7-904A-B2D3-16EA47682E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="289">
   <si>
     <t>Week</t>
   </si>
@@ -897,6 +897,12 @@
   </si>
   <si>
     <t>https://harmsm.github.io/physical-biochemistry/notes/23_diffusion-i.pdf</t>
+  </si>
+  <si>
+    <t>https://harmsm.github.io/physical-biochemistry/notes/24_diffusion-ii.pdf</t>
+  </si>
+  <si>
+    <t>24_notes</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1303,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2080,6 +2086,9 @@
       <c r="C27" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="F27" s="4" t="s">
+        <v>288</v>
+      </c>
       <c r="G27" t="s">
         <v>175</v>
       </c>
@@ -2230,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2624,6 +2633,14 @@
       </c>
       <c r="B48" s="12" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>288</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2648,6 +2665,7 @@
     <hyperlink ref="B47" r:id="rId18" xr:uid="{888CC1C3-1406-B947-895A-D16606A6EBAD}"/>
     <hyperlink ref="B19" r:id="rId19" xr:uid="{91AFF295-A0D2-D24C-9DAB-FD4BE8472086}"/>
     <hyperlink ref="B48" r:id="rId20" xr:uid="{7BC692B1-ADCF-1D4D-BE61-27FE315B3218}"/>
+    <hyperlink ref="B49" r:id="rId21" xr:uid="{24D16D87-F405-D648-B9F4-0B4AF33EA7D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added lab 8, updated schedle, updated homeworks
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C033D1C2-9AB7-904A-B2D3-16EA47682E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193F28FB-5CE7-6644-9EE7-1BD7CBD70774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="294">
   <si>
     <t>Week</t>
   </si>
@@ -903,6 +903,21 @@
   </si>
   <si>
     <t>24_notes</t>
+  </si>
+  <si>
+    <t>MoL, pp. 688-709</t>
+  </si>
+  <si>
+    <t>MoL pp. 787-802, MoL pp. 810-817</t>
+  </si>
+  <si>
+    <t>MoL pp. 688-709, 721-729</t>
+  </si>
+  <si>
+    <t>MoL pp. 709-718</t>
+  </si>
+  <si>
+    <t>MoL pp. 673-687</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1316,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1913,6 +1928,9 @@
       <c r="C21" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="E21" t="s">
+        <v>293</v>
+      </c>
       <c r="F21" t="s">
         <v>272</v>
       </c>
@@ -1973,6 +1991,9 @@
       <c r="C23" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="E23" s="4" t="s">
+        <v>292</v>
+      </c>
       <c r="F23" s="4" t="s">
         <v>280</v>
       </c>
@@ -1998,6 +2019,9 @@
       </c>
       <c r="C24" s="4" t="s">
         <v>130</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>282</v>
@@ -2060,6 +2084,9 @@
       </c>
       <c r="D26" t="s">
         <v>46</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>285</v>
@@ -2229,6 +2256,11 @@
       </c>
       <c r="C32" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated schedule with new link
</commit_message>
<xml_diff>
--- a/dev/schedule.xlsx
+++ b/dev/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/teaching/ch465_physical-biochemistry/physical-biochemistry/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B627BB-999D-9D45-9E57-652F34B7697E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E583340-05CD-7648-B38A-A4A350B01567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6AA3A7E9-13F9-C04B-9DBF-922EE8C7F601}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="300">
   <si>
     <t>Week</t>
   </si>
@@ -927,6 +927,15 @@
   </si>
   <si>
     <t>https://www.nature.com/articles/nrm.2017.7</t>
+  </si>
+  <si>
+    <t>rosen</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/22398450</t>
+  </si>
+  <si>
+    <t>hyman_rosen, rosen</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1337,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2179,7 +2188,7 @@
         <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>293</v>
@@ -2281,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C579E4-42EA-A04C-BB90-7E6AED047B2E}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2699,6 +2708,14 @@
       </c>
       <c r="B51" s="12" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>297</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2726,6 +2743,7 @@
     <hyperlink ref="B49" r:id="rId21" xr:uid="{24D16D87-F405-D648-B9F4-0B4AF33EA7D2}"/>
     <hyperlink ref="B50" r:id="rId22" xr:uid="{7A2B663D-5948-EE47-B4F4-FA030BE14395}"/>
     <hyperlink ref="B51" r:id="rId23" xr:uid="{A7075E40-C0D9-4045-AD2E-336E3870AB05}"/>
+    <hyperlink ref="B52" r:id="rId24" xr:uid="{CB1C7B4B-A5AE-BD48-B39F-FBC27E8EC352}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>